<commit_message>
add ca lam viec,..
</commit_message>
<xml_diff>
--- a/WHC_COVID_CHECK/WISOL.UI/DANH_SACH_TEST.xlsx
+++ b/WHC_COVID_CHECK/WISOL.UI/DANH_SACH_TEST.xlsx
@@ -15,7 +15,7 @@
     <sheet name="DATA" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DATA!$A$1:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DATA!$A$1:$G$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>STT</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Sảnh tầng 1, NM1</t>
+  </si>
+  <si>
+    <t>Ca làm việc</t>
   </si>
 </sst>
 </file>
@@ -487,21 +490,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -515,13 +518,16 @@
         <v>8</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -534,14 +540,15 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -554,15 +561,16 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F3"/>
+  <autoFilter ref="A1:G3"/>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="duplicateValues" dxfId="4" priority="106"/>
   </conditionalFormatting>

</xml_diff>